<commit_message>
DRAFT: State of my filesystem
</commit_message>
<xml_diff>
--- a/expectation.xlsx
+++ b/expectation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\IdeaProjects\nerdle_solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22CB445E-E6FE-4955-9EAB-5FB6F2F5D773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A3ED27-0CAB-41CD-B863-114071D32AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" xr2:uid="{8CE20E86-3072-48EB-9EB1-E5CD9B8DDA84}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Baseline</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Estimator</t>
+  </si>
+  <si>
+    <t>Only Possible</t>
+  </si>
+  <si>
+    <t>Algorithm</t>
   </si>
 </sst>
 </file>
@@ -403,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E0224A6-D493-4166-9D27-4D0FE5377F51}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,6 +421,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
       <c r="B1">
         <v>1</v>
       </c>
@@ -442,92 +451,122 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1223</v>
+        <v>1296</v>
       </c>
       <c r="D2">
-        <v>14425</v>
+        <v>14293</v>
       </c>
       <c r="E2">
-        <v>1431</v>
+        <v>1482</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
       </c>
       <c r="I2">
         <f>(B2*1+C2*2+D2*3+E2*4+F2*5+G2*6)/SUM(B2:G2)</f>
-        <v>3.0120608899297423</v>
+        <v>3.0117096018735361</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1258</v>
+        <v>1223</v>
       </c>
       <c r="D3">
-        <v>14261</v>
+        <v>14425</v>
       </c>
       <c r="E3">
-        <v>1560</v>
+        <v>1431</v>
       </c>
       <c r="I3">
         <f>(B3*1+C3*2+D3*3+E3*4+F3*5+G3*6)/SUM(B3:G3)</f>
-        <v>3.0175644028103044</v>
+        <v>3.0120608899297423</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>335</v>
+        <v>1258</v>
       </c>
       <c r="D4">
-        <v>14165</v>
+        <v>14261</v>
       </c>
       <c r="E4">
-        <v>2579</v>
+        <v>1560</v>
       </c>
       <c r="I4">
         <f>(B4*1+C4*2+D4*3+E4*4+F4*5+G4*6)/SUM(B4:G4)</f>
-        <v>3.1312646370023418</v>
+        <v>3.0175644028103044</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1445</v>
+        <v>1680</v>
       </c>
       <c r="D5">
-        <v>13862</v>
+        <v>13053</v>
       </c>
       <c r="E5">
-        <v>1758</v>
+        <v>2282</v>
       </c>
       <c r="F5">
-        <v>14</v>
+        <v>57</v>
+      </c>
+      <c r="G5">
+        <v>7</v>
       </c>
       <c r="I5">
         <f>(B5*1+C5*2+D5*3+E5*4+F5*5+G5*6)/SUM(B5:G5)</f>
-        <v>3.0198477751756441</v>
+        <v>3.043032786885246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>335</v>
+      </c>
+      <c r="D6">
+        <v>14165</v>
+      </c>
+      <c r="E6">
+        <v>2579</v>
+      </c>
+      <c r="I6">
+        <f>(B6*1+C6*2+D6*3+E6*4+F6*5+G6*6)/SUM(B6:G6)</f>
+        <v>3.1312646370023418</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I11">
+    <sortCondition ref="I2:I11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>